<commit_message>
Standardized names of variables, arguments and activities. Also, included more explanations in annotations.
</commit_message>
<xml_diff>
--- a/Test_Framework/_Tests.xlsx
+++ b/Test_Framework/_Tests.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8E0EBE-485C-478F-B60A-B47CD77F7485}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -61,12 +62,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -74,7 +75,7 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -82,8 +83,15 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -113,7 +121,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -390,19 +398,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="2" width="41.88671875" customWidth="1"/>
+    <col min="1" max="2" width="41.9140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="26.5" x14ac:dyDescent="0.8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -410,7 +416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -418,7 +424,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -426,7 +432,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -434,7 +440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -442,7 +448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -450,7 +456,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -458,7 +464,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -466,7 +472,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="13.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -474,7 +480,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="13.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -482,7 +488,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="13.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -490,7 +496,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="13.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -498,7 +504,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="13.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -506,7 +512,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="13.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -514,7 +520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="13.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -522,7 +528,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="13.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -530,7 +536,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="13.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -538,7 +544,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -546,7 +552,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="13.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -554,7 +560,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -563,8 +569,9 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B27" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Success,BRE,AppEx"</formula1>
     </dataValidation>
   </dataValidations>
@@ -574,22 +581,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="46.33203125" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1"/>
-    <col min="4" max="4" width="135.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.4140625" customWidth="1"/>
+    <col min="4" max="4" width="135.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="22.5" x14ac:dyDescent="0.65">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -603,7 +610,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -614,7 +621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -625,7 +632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -636,7 +643,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -647,7 +654,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -658,7 +665,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -669,7 +676,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -680,7 +687,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -691,7 +698,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -702,7 +709,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -713,7 +720,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -724,7 +731,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -735,7 +742,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -746,7 +753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -757,7 +764,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -768,7 +775,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -779,7 +786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -790,7 +797,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -801,7 +808,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -813,9 +820,10 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1"/>
+  <autoFilter ref="A1:D1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <phoneticPr fontId="3"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B28" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Success,BRE,AppEx"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>